<commit_message>
EPBDS-6033 Comparison with NaN is undefined, so > and < should return null
Equality operators like == and isXxx() are strong, so always should return true or false.

To unify meaning of isNaN(x) and x == NaN, NaN is equals to NaN, so NaN == NaN is true!
</commit_message>
<xml_diff>
--- a/STUDIO/org.openl.rules.test/test-resources/functionality/Miscs.xlsx
+++ b/STUDIO/org.openl.rules.test/test-resources/functionality/Miscs.xlsx
@@ -14,10 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="354" uniqueCount="54">
-  <si>
-    <t>A</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="358" uniqueCount="54">
   <si>
     <t>Step</t>
   </si>
@@ -176,6 +173,9 @@
   </si>
   <si>
     <t>-2147483648</t>
+  </si>
+  <si>
+    <t>Number</t>
   </si>
 </sst>
 </file>
@@ -518,8 +518,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B3:Q48"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A28" workbookViewId="0">
-      <selection activeCell="K47" sqref="K47"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="T23" sqref="T23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -537,60 +537,60 @@
   <sheetData>
     <row r="3" spans="2:17" x14ac:dyDescent="0.25">
       <c r="I3" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="4" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B4" s="2" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C4" s="2"/>
       <c r="I4" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="K4" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="L4" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="M4" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="L4" s="1" t="s">
+      <c r="N4" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="M4" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="N4" s="1" t="s">
-        <v>15</v>
-      </c>
       <c r="O4" t="s">
+        <v>24</v>
+      </c>
+      <c r="P4" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="P4" s="1" t="s">
+      <c r="Q4" t="s">
         <v>26</v>
-      </c>
-      <c r="Q4" t="s">
-        <v>27</v>
       </c>
     </row>
     <row r="5" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B5" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C5" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="I5" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="J5" t="s">
-        <v>0</v>
+        <v>53</v>
       </c>
       <c r="K5" t="s">
+        <v>11</v>
+      </c>
+      <c r="L5" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="M5" s="1" t="s">
         <v>12</v>
-      </c>
-      <c r="L5" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="M5" s="1" t="s">
-        <v>13</v>
       </c>
       <c r="O5">
         <v>1</v>
@@ -604,232 +604,232 @@
     </row>
     <row r="6" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B6" t="s">
+        <v>3</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="I6" t="s">
         <v>4</v>
       </c>
-      <c r="C6" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="I6" t="s">
-        <v>5</v>
-      </c>
       <c r="J6" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="K6" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="L6" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="M6" t="s">
-        <v>35</v>
+        <v>34</v>
+      </c>
+      <c r="N6" t="s">
+        <v>34</v>
       </c>
       <c r="O6" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="P6" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="Q6" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="7" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B7" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="I7" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="J7" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="K7" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="L7" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="M7" t="s">
+        <v>33</v>
+      </c>
+      <c r="N7" t="s">
         <v>34</v>
       </c>
       <c r="O7" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="P7" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="Q7" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="8" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B8" t="s">
+        <v>9</v>
+      </c>
+      <c r="C8" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="I8" t="s">
         <v>10</v>
       </c>
-      <c r="C8" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="I8" t="s">
-        <v>11</v>
-      </c>
       <c r="J8" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="K8" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="L8" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="M8" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="N8" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="O8" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="P8" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="Q8" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="9" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B9" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="I9" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="J9" t="s">
-        <v>25</v>
-      </c>
-      <c r="K9" t="s">
-        <v>35</v>
+        <v>24</v>
       </c>
       <c r="L9" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="M9" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="O9" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="P9" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="Q9" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="10" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B10" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="I10" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="J10" s="1" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="K10" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="L10" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="M10" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="N10" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="O10" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="P10" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="Q10" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="11" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B11" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="I11" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="J11" t="s">
-        <v>27</v>
-      </c>
-      <c r="K11" t="s">
-        <v>35</v>
+        <v>26</v>
       </c>
       <c r="L11" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="M11" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="O11" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="P11" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="Q11" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="12" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B12" t="s">
+        <v>41</v>
+      </c>
+      <c r="C12" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="C12" s="1" t="s">
+      <c r="I12" t="s">
         <v>43</v>
       </c>
-      <c r="I12" t="s">
+      <c r="J12" t="s">
         <v>44</v>
       </c>
-      <c r="J12" t="s">
+      <c r="K12" t="s">
+        <v>11</v>
+      </c>
+      <c r="L12" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="M12" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="O12" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="K12" t="s">
-        <v>12</v>
-      </c>
-      <c r="L12" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="M12" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="O12" s="1" t="s">
+      <c r="P12" s="1" t="s">
         <v>46</v>
       </c>
-      <c r="P12" s="1" t="s">
+      <c r="Q12" s="1" t="s">
         <v>47</v>
-      </c>
-      <c r="Q12" s="1" t="s">
-        <v>48</v>
       </c>
     </row>
     <row r="13" spans="2:17" x14ac:dyDescent="0.25">
@@ -837,60 +837,60 @@
     </row>
     <row r="15" spans="2:17" x14ac:dyDescent="0.25">
       <c r="I15" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="16" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B16" s="2" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C16" s="2"/>
       <c r="I16" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="K16" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="L16" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="M16" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="L16" s="1" t="s">
+      <c r="N16" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="M16" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="N16" s="1" t="s">
-        <v>15</v>
-      </c>
       <c r="O16" t="s">
+        <v>24</v>
+      </c>
+      <c r="P16" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="P16" s="1" t="s">
+      <c r="Q16" t="s">
         <v>26</v>
-      </c>
-      <c r="Q16" t="s">
-        <v>27</v>
       </c>
     </row>
     <row r="17" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B17" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C17" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="I17" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="J17" t="s">
-        <v>0</v>
+        <v>53</v>
       </c>
       <c r="K17" t="s">
+        <v>11</v>
+      </c>
+      <c r="L17" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="M17" s="1" t="s">
         <v>12</v>
-      </c>
-      <c r="L17" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="M17" s="1" t="s">
-        <v>13</v>
       </c>
       <c r="O17">
         <v>1</v>
@@ -904,290 +904,290 @@
     </row>
     <row r="18" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B18" t="s">
+        <v>3</v>
+      </c>
+      <c r="C18" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="I18" t="s">
         <v>4</v>
       </c>
-      <c r="C18" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="I18" t="s">
-        <v>5</v>
-      </c>
       <c r="J18" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="K18" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="L18" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="M18" t="s">
-        <v>35</v>
+        <v>34</v>
+      </c>
+      <c r="N18" t="s">
+        <v>34</v>
       </c>
       <c r="O18" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="P18" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="Q18" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="19" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B19" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C19" s="1" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="I19" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="J19" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="K19" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="L19" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="M19" t="s">
+        <v>33</v>
+      </c>
+      <c r="N19" t="s">
         <v>34</v>
       </c>
       <c r="O19" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="P19" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="Q19" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="20" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B20" t="s">
+        <v>9</v>
+      </c>
+      <c r="C20" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="I20" t="s">
         <v>10</v>
       </c>
-      <c r="C20" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="I20" t="s">
-        <v>11</v>
-      </c>
       <c r="J20" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="K20" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="L20" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="M20" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="N20" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="O20" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="P20" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="Q20" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="21" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B21" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C21" s="1" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="I21" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="J21" t="s">
-        <v>25</v>
-      </c>
-      <c r="K21" t="s">
-        <v>35</v>
+        <v>24</v>
       </c>
       <c r="L21" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="M21" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="O21" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="P21" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="Q21" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="22" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B22" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C22" s="1" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="I22" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="J22" s="1" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="K22" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="L22" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="M22" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="N22" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="O22" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="P22" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="Q22" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="23" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B23" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C23" s="1" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="I23" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="J23" t="s">
-        <v>27</v>
-      </c>
-      <c r="K23" t="s">
-        <v>35</v>
+        <v>26</v>
       </c>
       <c r="L23" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="M23" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="O23" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="P23" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="Q23" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="24" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B24" t="s">
+        <v>41</v>
+      </c>
+      <c r="C24" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="C24" s="1" t="s">
+      <c r="I24" t="s">
         <v>43</v>
       </c>
-      <c r="I24" t="s">
+      <c r="J24" t="s">
         <v>44</v>
       </c>
-      <c r="J24" t="s">
+      <c r="K24" t="s">
+        <v>11</v>
+      </c>
+      <c r="L24" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="M24" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="O24" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="K24" t="s">
-        <v>12</v>
-      </c>
-      <c r="L24" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="M24" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="O24" s="1" t="s">
+      <c r="P24" s="1" t="s">
         <v>46</v>
       </c>
-      <c r="P24" s="1" t="s">
+      <c r="Q24" s="1" t="s">
         <v>47</v>
-      </c>
-      <c r="Q24" s="1" t="s">
-        <v>48</v>
       </c>
     </row>
     <row r="27" spans="2:17" x14ac:dyDescent="0.25">
       <c r="I27" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="28" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B28" s="2" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="C28" s="2"/>
       <c r="I28" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="K28" s="1" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="L28" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="M28" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="N28" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="M28" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="N28" s="1" t="s">
-        <v>15</v>
-      </c>
       <c r="O28" t="s">
+        <v>24</v>
+      </c>
+      <c r="P28" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="P28" s="1" t="s">
+      <c r="Q28" t="s">
         <v>26</v>
-      </c>
-      <c r="Q28" t="s">
-        <v>27</v>
       </c>
     </row>
     <row r="29" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B29" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C29" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="I29" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="J29" t="s">
-        <v>0</v>
+        <v>53</v>
       </c>
       <c r="K29" s="1" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="L29" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="M29" s="1" t="s">
         <v>49</v>
-      </c>
-      <c r="M29" s="1" t="s">
-        <v>50</v>
       </c>
       <c r="O29">
         <v>1</v>
@@ -1201,284 +1201,290 @@
     </row>
     <row r="30" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B30" t="s">
+        <v>3</v>
+      </c>
+      <c r="C30" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="I30" t="s">
         <v>4</v>
       </c>
-      <c r="C30" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="I30" t="s">
-        <v>5</v>
-      </c>
       <c r="J30" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="K30" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="L30" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="M30" t="s">
-        <v>35</v>
+        <v>34</v>
+      </c>
+      <c r="N30" t="s">
+        <v>34</v>
       </c>
       <c r="O30" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="P30" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="Q30" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="31" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B31" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C31" s="1" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="I31" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="J31" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="K31" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="L31" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="M31" t="s">
+        <v>33</v>
+      </c>
+      <c r="N31" t="s">
         <v>34</v>
       </c>
       <c r="O31" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="P31" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="Q31" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="32" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B32" t="s">
+        <v>9</v>
+      </c>
+      <c r="C32" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="I32" t="s">
         <v>10</v>
       </c>
-      <c r="C32" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="I32" t="s">
-        <v>11</v>
-      </c>
       <c r="J32" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="K32" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="L32" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="M32" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="N32" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="O32" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="P32" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="Q32" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="33" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B33" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C33" s="1" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="I33" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="J33" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="K33" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="L33" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="M33" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="O33" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="P33" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="Q33" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="34" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B34" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C34" s="1" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="I34" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="J34" s="1" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="K34" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="L34" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="M34" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="N34" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="O34" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="P34" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="Q34" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="35" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B35" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C35" s="1" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="I35" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="J35" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="K35" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="L35" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="M35" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="O35" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="P35" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="Q35" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="36" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B36" t="s">
+        <v>41</v>
+      </c>
+      <c r="C36" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="C36" s="1" t="s">
+      <c r="I36" t="s">
         <v>43</v>
       </c>
-      <c r="I36" t="s">
+      <c r="J36" t="s">
         <v>44</v>
       </c>
-      <c r="J36" t="s">
+      <c r="K36" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="L36" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="M36" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="O36" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="K36" s="1" t="s">
+      <c r="P36" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="Q36" s="1" t="s">
         <v>47</v>
-      </c>
-      <c r="L36" s="1" t="s">
-        <v>49</v>
-      </c>
-      <c r="M36" s="1" t="s">
-        <v>50</v>
-      </c>
-      <c r="O36" s="1" t="s">
-        <v>46</v>
-      </c>
-      <c r="P36" s="1" t="s">
-        <v>47</v>
-      </c>
-      <c r="Q36" s="1" t="s">
-        <v>48</v>
       </c>
     </row>
     <row r="39" spans="2:17" x14ac:dyDescent="0.25">
       <c r="I39" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="40" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B40" s="2" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C40" s="2"/>
       <c r="I40" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="K40" s="1" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="L40" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="M40" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="N40" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="M40" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="N40" s="1" t="s">
-        <v>15</v>
-      </c>
       <c r="O40" t="s">
+        <v>24</v>
+      </c>
+      <c r="P40" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="P40" s="1" t="s">
+      <c r="Q40" t="s">
         <v>26</v>
-      </c>
-      <c r="Q40" t="s">
-        <v>27</v>
       </c>
     </row>
     <row r="41" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B41" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C41" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="I41" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="J41" t="s">
-        <v>0</v>
+        <v>53</v>
       </c>
       <c r="K41" s="1" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="L41" s="1">
         <v>2147483647</v>
@@ -1498,232 +1504,238 @@
     </row>
     <row r="42" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B42" t="s">
+        <v>3</v>
+      </c>
+      <c r="C42" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="I42" t="s">
         <v>4</v>
       </c>
-      <c r="C42" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="I42" t="s">
-        <v>5</v>
-      </c>
       <c r="J42" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="K42" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="L42" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="M42" t="s">
-        <v>35</v>
+        <v>34</v>
+      </c>
+      <c r="N42" t="s">
+        <v>34</v>
       </c>
       <c r="O42" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="P42" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="Q42" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="43" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B43" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C43" s="1" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="I43" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="J43" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="K43" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="L43" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="M43" t="s">
+        <v>33</v>
+      </c>
+      <c r="N43" t="s">
         <v>34</v>
       </c>
       <c r="O43" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="P43" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="Q43" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="44" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B44" t="s">
+        <v>9</v>
+      </c>
+      <c r="C44" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="I44" t="s">
         <v>10</v>
       </c>
-      <c r="C44" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="I44" t="s">
-        <v>11</v>
-      </c>
       <c r="J44" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="K44" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="L44" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="M44" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="N44" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="O44" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="P44" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="Q44" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="45" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B45" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C45" s="1" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="I45" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="J45" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="K45" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="L45" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="M45" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="O45" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="P45" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="Q45" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="46" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B46" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C46" s="1" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="I46" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="J46" s="1" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="K46" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="L46" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="M46" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="N46" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="O46" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="P46" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="Q46" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="47" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B47" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C47" s="1" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="I47" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="J47" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="K47" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="L47" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="M47" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="O47" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="P47" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="Q47" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="48" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B48" t="s">
+        <v>41</v>
+      </c>
+      <c r="C48" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="C48" s="1" t="s">
+      <c r="I48" t="s">
         <v>43</v>
       </c>
-      <c r="I48" t="s">
+      <c r="J48" t="s">
         <v>44</v>
       </c>
-      <c r="J48" t="s">
+      <c r="K48" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="L48" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="M48" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="O48" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="K48" s="1" t="s">
+      <c r="P48" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="Q48" s="1" t="s">
         <v>47</v>
-      </c>
-      <c r="L48" s="1" t="s">
-        <v>52</v>
-      </c>
-      <c r="M48" s="1" t="s">
-        <v>53</v>
-      </c>
-      <c r="O48" s="1" t="s">
-        <v>46</v>
-      </c>
-      <c r="P48" s="1" t="s">
-        <v>47</v>
-      </c>
-      <c r="Q48" s="1" t="s">
-        <v>48</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
EPBDS-12566 Add methods Numbers.toString() for number formatting
</commit_message>
<xml_diff>
--- a/STUDIO/org.openl.rules.test/test-resources/functionality/Miscs.xlsx
+++ b/STUDIO/org.openl.rules.test/test-resources/functionality/Miscs.xlsx
@@ -1,10 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="10111"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A6DF9C87-F16E-2F4F-928F-FDBC94352A3B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="38400" windowHeight="21600" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -14,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="358" uniqueCount="54">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="358" uniqueCount="56">
   <si>
     <t>Step</t>
   </si>
@@ -176,12 +177,18 @@
   </si>
   <si>
     <t>Number</t>
+  </si>
+  <si>
+    <t>∞</t>
+  </si>
+  <si>
+    <t>-∞</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -224,6 +231,9 @@
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
     </ext>
   </extLst>
 </styleSheet>
@@ -272,7 +282,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -305,9 +315,26 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -340,6 +367,23 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -515,32 +559,32 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="B3:Q48"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="T23" sqref="T23"/>
+      <selection activeCell="M23" sqref="M23"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="2" max="2" width="10.5703125" customWidth="1"/>
-    <col min="3" max="3" width="12.85546875" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="15.7109375" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="8.5703125" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="4.85546875" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="20.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.5" customWidth="1"/>
+    <col min="3" max="3" width="12.83203125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="15.6640625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="8.5" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="4.83203125" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="20.33203125" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="21" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="6.5703125" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="6.5" bestFit="1" customWidth="1"/>
     <col min="15" max="17" width="3" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="2:17" x14ac:dyDescent="0.25">
+    <row r="3" spans="2:17" x14ac:dyDescent="0.2">
       <c r="I3" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="2:17" x14ac:dyDescent="0.25">
+    <row r="4" spans="2:17" x14ac:dyDescent="0.2">
       <c r="B4" s="2" t="s">
         <v>17</v>
       </c>
@@ -570,7 +614,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="5" spans="2:17" x14ac:dyDescent="0.25">
+    <row r="5" spans="2:17" x14ac:dyDescent="0.2">
       <c r="B5" t="s">
         <v>0</v>
       </c>
@@ -602,7 +646,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="6" spans="2:17" x14ac:dyDescent="0.25">
+    <row r="6" spans="2:17" x14ac:dyDescent="0.2">
       <c r="B6" t="s">
         <v>3</v>
       </c>
@@ -637,7 +681,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="7" spans="2:17" x14ac:dyDescent="0.25">
+    <row r="7" spans="2:17" x14ac:dyDescent="0.2">
       <c r="B7" t="s">
         <v>8</v>
       </c>
@@ -672,7 +716,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="8" spans="2:17" x14ac:dyDescent="0.25">
+    <row r="8" spans="2:17" x14ac:dyDescent="0.2">
       <c r="B8" t="s">
         <v>9</v>
       </c>
@@ -707,7 +751,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="9" spans="2:17" x14ac:dyDescent="0.25">
+    <row r="9" spans="2:17" x14ac:dyDescent="0.2">
       <c r="B9" t="s">
         <v>27</v>
       </c>
@@ -736,7 +780,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="10" spans="2:17" x14ac:dyDescent="0.25">
+    <row r="10" spans="2:17" x14ac:dyDescent="0.2">
       <c r="B10" t="s">
         <v>16</v>
       </c>
@@ -771,7 +815,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="11" spans="2:17" x14ac:dyDescent="0.25">
+    <row r="11" spans="2:17" x14ac:dyDescent="0.2">
       <c r="B11" t="s">
         <v>28</v>
       </c>
@@ -800,7 +844,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="12" spans="2:17" x14ac:dyDescent="0.25">
+    <row r="12" spans="2:17" x14ac:dyDescent="0.2">
       <c r="B12" t="s">
         <v>41</v>
       </c>
@@ -817,10 +861,10 @@
         <v>11</v>
       </c>
       <c r="L12" s="1" t="s">
-        <v>15</v>
+        <v>54</v>
       </c>
       <c r="M12" s="1" t="s">
-        <v>12</v>
+        <v>55</v>
       </c>
       <c r="O12" s="1" t="s">
         <v>45</v>
@@ -832,15 +876,15 @@
         <v>47</v>
       </c>
     </row>
-    <row r="13" spans="2:17" x14ac:dyDescent="0.25">
+    <row r="13" spans="2:17" x14ac:dyDescent="0.2">
       <c r="C13" s="1"/>
     </row>
-    <row r="15" spans="2:17" x14ac:dyDescent="0.25">
+    <row r="15" spans="2:17" x14ac:dyDescent="0.2">
       <c r="I15" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="16" spans="2:17" x14ac:dyDescent="0.25">
+    <row r="16" spans="2:17" x14ac:dyDescent="0.2">
       <c r="B16" s="2" t="s">
         <v>36</v>
       </c>
@@ -870,7 +914,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="17" spans="2:17" x14ac:dyDescent="0.25">
+    <row r="17" spans="2:17" x14ac:dyDescent="0.2">
       <c r="B17" t="s">
         <v>0</v>
       </c>
@@ -902,7 +946,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="18" spans="2:17" x14ac:dyDescent="0.25">
+    <row r="18" spans="2:17" x14ac:dyDescent="0.2">
       <c r="B18" t="s">
         <v>3</v>
       </c>
@@ -937,7 +981,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="19" spans="2:17" x14ac:dyDescent="0.25">
+    <row r="19" spans="2:17" x14ac:dyDescent="0.2">
       <c r="B19" t="s">
         <v>8</v>
       </c>
@@ -972,7 +1016,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="20" spans="2:17" x14ac:dyDescent="0.25">
+    <row r="20" spans="2:17" x14ac:dyDescent="0.2">
       <c r="B20" t="s">
         <v>9</v>
       </c>
@@ -1007,7 +1051,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="21" spans="2:17" x14ac:dyDescent="0.25">
+    <row r="21" spans="2:17" x14ac:dyDescent="0.2">
       <c r="B21" t="s">
         <v>27</v>
       </c>
@@ -1036,7 +1080,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="22" spans="2:17" x14ac:dyDescent="0.25">
+    <row r="22" spans="2:17" x14ac:dyDescent="0.2">
       <c r="B22" t="s">
         <v>16</v>
       </c>
@@ -1071,7 +1115,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="23" spans="2:17" x14ac:dyDescent="0.25">
+    <row r="23" spans="2:17" x14ac:dyDescent="0.2">
       <c r="B23" t="s">
         <v>28</v>
       </c>
@@ -1100,7 +1144,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="24" spans="2:17" x14ac:dyDescent="0.25">
+    <row r="24" spans="2:17" x14ac:dyDescent="0.2">
       <c r="B24" t="s">
         <v>41</v>
       </c>
@@ -1117,10 +1161,10 @@
         <v>11</v>
       </c>
       <c r="L24" s="1" t="s">
-        <v>15</v>
+        <v>54</v>
       </c>
       <c r="M24" s="1" t="s">
-        <v>12</v>
+        <v>55</v>
       </c>
       <c r="O24" s="1" t="s">
         <v>45</v>
@@ -1132,12 +1176,12 @@
         <v>47</v>
       </c>
     </row>
-    <row r="27" spans="2:17" x14ac:dyDescent="0.25">
+    <row r="27" spans="2:17" x14ac:dyDescent="0.2">
       <c r="I27" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="28" spans="2:17" x14ac:dyDescent="0.25">
+    <row r="28" spans="2:17" x14ac:dyDescent="0.2">
       <c r="B28" s="2" t="s">
         <v>37</v>
       </c>
@@ -1167,7 +1211,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="29" spans="2:17" x14ac:dyDescent="0.25">
+    <row r="29" spans="2:17" x14ac:dyDescent="0.2">
       <c r="B29" t="s">
         <v>0</v>
       </c>
@@ -1199,7 +1243,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="30" spans="2:17" x14ac:dyDescent="0.25">
+    <row r="30" spans="2:17" x14ac:dyDescent="0.2">
       <c r="B30" t="s">
         <v>3</v>
       </c>
@@ -1234,7 +1278,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="31" spans="2:17" x14ac:dyDescent="0.25">
+    <row r="31" spans="2:17" x14ac:dyDescent="0.2">
       <c r="B31" t="s">
         <v>8</v>
       </c>
@@ -1269,7 +1313,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="32" spans="2:17" x14ac:dyDescent="0.25">
+    <row r="32" spans="2:17" x14ac:dyDescent="0.2">
       <c r="B32" t="s">
         <v>9</v>
       </c>
@@ -1304,7 +1348,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="33" spans="2:17" x14ac:dyDescent="0.25">
+    <row r="33" spans="2:17" x14ac:dyDescent="0.2">
       <c r="B33" t="s">
         <v>27</v>
       </c>
@@ -1336,7 +1380,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="34" spans="2:17" x14ac:dyDescent="0.25">
+    <row r="34" spans="2:17" x14ac:dyDescent="0.2">
       <c r="B34" t="s">
         <v>16</v>
       </c>
@@ -1371,7 +1415,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="35" spans="2:17" x14ac:dyDescent="0.25">
+    <row r="35" spans="2:17" x14ac:dyDescent="0.2">
       <c r="B35" t="s">
         <v>28</v>
       </c>
@@ -1403,7 +1447,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="36" spans="2:17" x14ac:dyDescent="0.25">
+    <row r="36" spans="2:17" x14ac:dyDescent="0.2">
       <c r="B36" t="s">
         <v>41</v>
       </c>
@@ -1435,12 +1479,12 @@
         <v>47</v>
       </c>
     </row>
-    <row r="39" spans="2:17" x14ac:dyDescent="0.25">
+    <row r="39" spans="2:17" x14ac:dyDescent="0.2">
       <c r="I39" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="40" spans="2:17" x14ac:dyDescent="0.25">
+    <row r="40" spans="2:17" x14ac:dyDescent="0.2">
       <c r="B40" s="2" t="s">
         <v>40</v>
       </c>
@@ -1470,7 +1514,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="41" spans="2:17" x14ac:dyDescent="0.25">
+    <row r="41" spans="2:17" x14ac:dyDescent="0.2">
       <c r="B41" t="s">
         <v>0</v>
       </c>
@@ -1502,7 +1546,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="42" spans="2:17" x14ac:dyDescent="0.25">
+    <row r="42" spans="2:17" x14ac:dyDescent="0.2">
       <c r="B42" t="s">
         <v>3</v>
       </c>
@@ -1537,7 +1581,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="43" spans="2:17" x14ac:dyDescent="0.25">
+    <row r="43" spans="2:17" x14ac:dyDescent="0.2">
       <c r="B43" t="s">
         <v>8</v>
       </c>
@@ -1572,7 +1616,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="44" spans="2:17" x14ac:dyDescent="0.25">
+    <row r="44" spans="2:17" x14ac:dyDescent="0.2">
       <c r="B44" t="s">
         <v>9</v>
       </c>
@@ -1607,7 +1651,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="45" spans="2:17" x14ac:dyDescent="0.25">
+    <row r="45" spans="2:17" x14ac:dyDescent="0.2">
       <c r="B45" t="s">
         <v>27</v>
       </c>
@@ -1639,7 +1683,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="46" spans="2:17" x14ac:dyDescent="0.25">
+    <row r="46" spans="2:17" x14ac:dyDescent="0.2">
       <c r="B46" t="s">
         <v>16</v>
       </c>
@@ -1674,7 +1718,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="47" spans="2:17" x14ac:dyDescent="0.25">
+    <row r="47" spans="2:17" x14ac:dyDescent="0.2">
       <c r="B47" t="s">
         <v>28</v>
       </c>
@@ -1706,7 +1750,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="48" spans="2:17" x14ac:dyDescent="0.25">
+    <row r="48" spans="2:17" x14ac:dyDescent="0.2">
       <c r="B48" t="s">
         <v>41</v>
       </c>

</xml_diff>

<commit_message>
EPBDS-12566 Add methods Numbers.toString() for number formatting (#392)
</commit_message>
<xml_diff>
--- a/STUDIO/org.openl.rules.test/test-resources/functionality/Miscs.xlsx
+++ b/STUDIO/org.openl.rules.test/test-resources/functionality/Miscs.xlsx
@@ -1,10 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="10111"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A6DF9C87-F16E-2F4F-928F-FDBC94352A3B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="38400" windowHeight="21600" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -14,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="358" uniqueCount="54">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="358" uniqueCount="56">
   <si>
     <t>Step</t>
   </si>
@@ -176,12 +177,18 @@
   </si>
   <si>
     <t>Number</t>
+  </si>
+  <si>
+    <t>∞</t>
+  </si>
+  <si>
+    <t>-∞</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -224,6 +231,9 @@
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
     </ext>
   </extLst>
 </styleSheet>
@@ -272,7 +282,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -305,9 +315,26 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -340,6 +367,23 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -515,32 +559,32 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="B3:Q48"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="T23" sqref="T23"/>
+      <selection activeCell="M23" sqref="M23"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="2" max="2" width="10.5703125" customWidth="1"/>
-    <col min="3" max="3" width="12.85546875" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="15.7109375" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="8.5703125" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="4.85546875" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="20.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.5" customWidth="1"/>
+    <col min="3" max="3" width="12.83203125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="15.6640625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="8.5" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="4.83203125" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="20.33203125" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="21" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="6.5703125" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="6.5" bestFit="1" customWidth="1"/>
     <col min="15" max="17" width="3" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="2:17" x14ac:dyDescent="0.25">
+    <row r="3" spans="2:17" x14ac:dyDescent="0.2">
       <c r="I3" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="2:17" x14ac:dyDescent="0.25">
+    <row r="4" spans="2:17" x14ac:dyDescent="0.2">
       <c r="B4" s="2" t="s">
         <v>17</v>
       </c>
@@ -570,7 +614,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="5" spans="2:17" x14ac:dyDescent="0.25">
+    <row r="5" spans="2:17" x14ac:dyDescent="0.2">
       <c r="B5" t="s">
         <v>0</v>
       </c>
@@ -602,7 +646,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="6" spans="2:17" x14ac:dyDescent="0.25">
+    <row r="6" spans="2:17" x14ac:dyDescent="0.2">
       <c r="B6" t="s">
         <v>3</v>
       </c>
@@ -637,7 +681,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="7" spans="2:17" x14ac:dyDescent="0.25">
+    <row r="7" spans="2:17" x14ac:dyDescent="0.2">
       <c r="B7" t="s">
         <v>8</v>
       </c>
@@ -672,7 +716,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="8" spans="2:17" x14ac:dyDescent="0.25">
+    <row r="8" spans="2:17" x14ac:dyDescent="0.2">
       <c r="B8" t="s">
         <v>9</v>
       </c>
@@ -707,7 +751,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="9" spans="2:17" x14ac:dyDescent="0.25">
+    <row r="9" spans="2:17" x14ac:dyDescent="0.2">
       <c r="B9" t="s">
         <v>27</v>
       </c>
@@ -736,7 +780,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="10" spans="2:17" x14ac:dyDescent="0.25">
+    <row r="10" spans="2:17" x14ac:dyDescent="0.2">
       <c r="B10" t="s">
         <v>16</v>
       </c>
@@ -771,7 +815,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="11" spans="2:17" x14ac:dyDescent="0.25">
+    <row r="11" spans="2:17" x14ac:dyDescent="0.2">
       <c r="B11" t="s">
         <v>28</v>
       </c>
@@ -800,7 +844,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="12" spans="2:17" x14ac:dyDescent="0.25">
+    <row r="12" spans="2:17" x14ac:dyDescent="0.2">
       <c r="B12" t="s">
         <v>41</v>
       </c>
@@ -817,10 +861,10 @@
         <v>11</v>
       </c>
       <c r="L12" s="1" t="s">
-        <v>15</v>
+        <v>54</v>
       </c>
       <c r="M12" s="1" t="s">
-        <v>12</v>
+        <v>55</v>
       </c>
       <c r="O12" s="1" t="s">
         <v>45</v>
@@ -832,15 +876,15 @@
         <v>47</v>
       </c>
     </row>
-    <row r="13" spans="2:17" x14ac:dyDescent="0.25">
+    <row r="13" spans="2:17" x14ac:dyDescent="0.2">
       <c r="C13" s="1"/>
     </row>
-    <row r="15" spans="2:17" x14ac:dyDescent="0.25">
+    <row r="15" spans="2:17" x14ac:dyDescent="0.2">
       <c r="I15" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="16" spans="2:17" x14ac:dyDescent="0.25">
+    <row r="16" spans="2:17" x14ac:dyDescent="0.2">
       <c r="B16" s="2" t="s">
         <v>36</v>
       </c>
@@ -870,7 +914,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="17" spans="2:17" x14ac:dyDescent="0.25">
+    <row r="17" spans="2:17" x14ac:dyDescent="0.2">
       <c r="B17" t="s">
         <v>0</v>
       </c>
@@ -902,7 +946,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="18" spans="2:17" x14ac:dyDescent="0.25">
+    <row r="18" spans="2:17" x14ac:dyDescent="0.2">
       <c r="B18" t="s">
         <v>3</v>
       </c>
@@ -937,7 +981,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="19" spans="2:17" x14ac:dyDescent="0.25">
+    <row r="19" spans="2:17" x14ac:dyDescent="0.2">
       <c r="B19" t="s">
         <v>8</v>
       </c>
@@ -972,7 +1016,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="20" spans="2:17" x14ac:dyDescent="0.25">
+    <row r="20" spans="2:17" x14ac:dyDescent="0.2">
       <c r="B20" t="s">
         <v>9</v>
       </c>
@@ -1007,7 +1051,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="21" spans="2:17" x14ac:dyDescent="0.25">
+    <row r="21" spans="2:17" x14ac:dyDescent="0.2">
       <c r="B21" t="s">
         <v>27</v>
       </c>
@@ -1036,7 +1080,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="22" spans="2:17" x14ac:dyDescent="0.25">
+    <row r="22" spans="2:17" x14ac:dyDescent="0.2">
       <c r="B22" t="s">
         <v>16</v>
       </c>
@@ -1071,7 +1115,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="23" spans="2:17" x14ac:dyDescent="0.25">
+    <row r="23" spans="2:17" x14ac:dyDescent="0.2">
       <c r="B23" t="s">
         <v>28</v>
       </c>
@@ -1100,7 +1144,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="24" spans="2:17" x14ac:dyDescent="0.25">
+    <row r="24" spans="2:17" x14ac:dyDescent="0.2">
       <c r="B24" t="s">
         <v>41</v>
       </c>
@@ -1117,10 +1161,10 @@
         <v>11</v>
       </c>
       <c r="L24" s="1" t="s">
-        <v>15</v>
+        <v>54</v>
       </c>
       <c r="M24" s="1" t="s">
-        <v>12</v>
+        <v>55</v>
       </c>
       <c r="O24" s="1" t="s">
         <v>45</v>
@@ -1132,12 +1176,12 @@
         <v>47</v>
       </c>
     </row>
-    <row r="27" spans="2:17" x14ac:dyDescent="0.25">
+    <row r="27" spans="2:17" x14ac:dyDescent="0.2">
       <c r="I27" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="28" spans="2:17" x14ac:dyDescent="0.25">
+    <row r="28" spans="2:17" x14ac:dyDescent="0.2">
       <c r="B28" s="2" t="s">
         <v>37</v>
       </c>
@@ -1167,7 +1211,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="29" spans="2:17" x14ac:dyDescent="0.25">
+    <row r="29" spans="2:17" x14ac:dyDescent="0.2">
       <c r="B29" t="s">
         <v>0</v>
       </c>
@@ -1199,7 +1243,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="30" spans="2:17" x14ac:dyDescent="0.25">
+    <row r="30" spans="2:17" x14ac:dyDescent="0.2">
       <c r="B30" t="s">
         <v>3</v>
       </c>
@@ -1234,7 +1278,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="31" spans="2:17" x14ac:dyDescent="0.25">
+    <row r="31" spans="2:17" x14ac:dyDescent="0.2">
       <c r="B31" t="s">
         <v>8</v>
       </c>
@@ -1269,7 +1313,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="32" spans="2:17" x14ac:dyDescent="0.25">
+    <row r="32" spans="2:17" x14ac:dyDescent="0.2">
       <c r="B32" t="s">
         <v>9</v>
       </c>
@@ -1304,7 +1348,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="33" spans="2:17" x14ac:dyDescent="0.25">
+    <row r="33" spans="2:17" x14ac:dyDescent="0.2">
       <c r="B33" t="s">
         <v>27</v>
       </c>
@@ -1336,7 +1380,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="34" spans="2:17" x14ac:dyDescent="0.25">
+    <row r="34" spans="2:17" x14ac:dyDescent="0.2">
       <c r="B34" t="s">
         <v>16</v>
       </c>
@@ -1371,7 +1415,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="35" spans="2:17" x14ac:dyDescent="0.25">
+    <row r="35" spans="2:17" x14ac:dyDescent="0.2">
       <c r="B35" t="s">
         <v>28</v>
       </c>
@@ -1403,7 +1447,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="36" spans="2:17" x14ac:dyDescent="0.25">
+    <row r="36" spans="2:17" x14ac:dyDescent="0.2">
       <c r="B36" t="s">
         <v>41</v>
       </c>
@@ -1435,12 +1479,12 @@
         <v>47</v>
       </c>
     </row>
-    <row r="39" spans="2:17" x14ac:dyDescent="0.25">
+    <row r="39" spans="2:17" x14ac:dyDescent="0.2">
       <c r="I39" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="40" spans="2:17" x14ac:dyDescent="0.25">
+    <row r="40" spans="2:17" x14ac:dyDescent="0.2">
       <c r="B40" s="2" t="s">
         <v>40</v>
       </c>
@@ -1470,7 +1514,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="41" spans="2:17" x14ac:dyDescent="0.25">
+    <row r="41" spans="2:17" x14ac:dyDescent="0.2">
       <c r="B41" t="s">
         <v>0</v>
       </c>
@@ -1502,7 +1546,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="42" spans="2:17" x14ac:dyDescent="0.25">
+    <row r="42" spans="2:17" x14ac:dyDescent="0.2">
       <c r="B42" t="s">
         <v>3</v>
       </c>
@@ -1537,7 +1581,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="43" spans="2:17" x14ac:dyDescent="0.25">
+    <row r="43" spans="2:17" x14ac:dyDescent="0.2">
       <c r="B43" t="s">
         <v>8</v>
       </c>
@@ -1572,7 +1616,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="44" spans="2:17" x14ac:dyDescent="0.25">
+    <row r="44" spans="2:17" x14ac:dyDescent="0.2">
       <c r="B44" t="s">
         <v>9</v>
       </c>
@@ -1607,7 +1651,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="45" spans="2:17" x14ac:dyDescent="0.25">
+    <row r="45" spans="2:17" x14ac:dyDescent="0.2">
       <c r="B45" t="s">
         <v>27</v>
       </c>
@@ -1639,7 +1683,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="46" spans="2:17" x14ac:dyDescent="0.25">
+    <row r="46" spans="2:17" x14ac:dyDescent="0.2">
       <c r="B46" t="s">
         <v>16</v>
       </c>
@@ -1674,7 +1718,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="47" spans="2:17" x14ac:dyDescent="0.25">
+    <row r="47" spans="2:17" x14ac:dyDescent="0.2">
       <c r="B47" t="s">
         <v>28</v>
       </c>
@@ -1706,7 +1750,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="48" spans="2:17" x14ac:dyDescent="0.25">
+    <row r="48" spans="2:17" x14ac:dyDescent="0.2">
       <c r="B48" t="s">
         <v>41</v>
       </c>

</xml_diff>